<commit_message>
excel file design finished
</commit_message>
<xml_diff>
--- a/proj/output/1401CE04.xlsx
+++ b/proj/output/1401CE04.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -40,6 +40,21 @@
       <b val="1"/>
       <sz val="12"/>
     </font>
+    <font>
+      <name val="Century"/>
+      <color rgb="00008000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Century"/>
+      <color rgb="000000FF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Century"/>
+      <color rgb="00FF0000"/>
+      <sz val="12"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -49,7 +64,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -58,11 +73,17 @@
       <diagonal/>
     </border>
     <border/>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
@@ -72,6 +93,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -468,7 +504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A5:E7"/>
+  <dimension ref="A5:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +560,433 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n"/>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>Wrong</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>Not Attempt</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>No.</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>Marking</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>105</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D12" s="4" t="n"/>
+      <c r="E12" s="7" t="inlineStr">
+        <is>
+          <t>104/140</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>Student Ans</t>
+        </is>
+      </c>
+      <c r="B15" s="8" t="inlineStr">
+        <is>
+          <t>Correct Ans</t>
+        </is>
+      </c>
+      <c r="D15" s="8" t="inlineStr">
+        <is>
+          <t>Student Ans</t>
+        </is>
+      </c>
+      <c r="E15" s="8" t="inlineStr">
+        <is>
+          <t>Correct Ans</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr"/>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="E17" s="7" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+      <c r="D18" s="6" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+      <c r="E18" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr"/>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="B22" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr"/>
+      <c r="B24" s="7" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+      <c r="B25" s="7" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B26" s="7" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+      <c r="B27" s="7" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="B28" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr"/>
+      <c r="B29" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+      <c r="B30" s="7" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr"/>
+      <c r="B31" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B32" s="7" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="B33" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="5" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+      <c r="B34" s="7" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="B35" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+      <c r="B36" s="7" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr"/>
+      <c r="B37" s="7" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="5" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+      <c r="B38" s="7" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="B39" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="B40" s="7" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A5:E5"/>

</xml_diff>